<commit_message>
esta si funciona pre
</commit_message>
<xml_diff>
--- a/datos_kwh_costa_caribe.xlsx
+++ b/datos_kwh_costa_caribe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\astri\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BEF7517-B816-414F-9BF3-AFA267DC3210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136FEC08-4B5B-4803-9513-D31ADA64576D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4236" yWindow="1116" windowWidth="17280" windowHeight="8880" xr2:uid="{F1EBCE9C-3D6C-4EA4-96FD-4A7A0EAFCF3C}"/>
   </bookViews>
@@ -429,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{940C0B72-C9B5-4EB8-944E-6D5C34C82158}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -736,6 +736,558 @@
         <v>1180.3</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>44927</v>
+      </c>
+      <c r="B14">
+        <v>0.23</v>
+      </c>
+      <c r="C14">
+        <v>200.1</v>
+      </c>
+      <c r="D14">
+        <v>27.5</v>
+      </c>
+      <c r="E14">
+        <v>420.5</v>
+      </c>
+      <c r="F14">
+        <v>280.3</v>
+      </c>
+      <c r="G14">
+        <v>1150.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>44958</v>
+      </c>
+      <c r="B15">
+        <v>0.22</v>
+      </c>
+      <c r="C15">
+        <v>180.5</v>
+      </c>
+      <c r="D15">
+        <v>28</v>
+      </c>
+      <c r="E15">
+        <v>450.7</v>
+      </c>
+      <c r="F15">
+        <v>300.5</v>
+      </c>
+      <c r="G15">
+        <v>1180.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>44986</v>
+      </c>
+      <c r="B16">
+        <v>0.24</v>
+      </c>
+      <c r="C16">
+        <v>150</v>
+      </c>
+      <c r="D16">
+        <v>28.5</v>
+      </c>
+      <c r="E16">
+        <v>480.2</v>
+      </c>
+      <c r="F16">
+        <v>320</v>
+      </c>
+      <c r="G16">
+        <v>1200.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>45017</v>
+      </c>
+      <c r="B17">
+        <v>0.25</v>
+      </c>
+      <c r="C17">
+        <v>120.3</v>
+      </c>
+      <c r="D17">
+        <v>29</v>
+      </c>
+      <c r="E17">
+        <v>500</v>
+      </c>
+      <c r="F17">
+        <v>330.2</v>
+      </c>
+      <c r="G17">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>45047</v>
+      </c>
+      <c r="B18">
+        <v>0.26</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+      <c r="D18">
+        <v>29.5</v>
+      </c>
+      <c r="E18">
+        <v>520.5</v>
+      </c>
+      <c r="F18">
+        <v>340.5</v>
+      </c>
+      <c r="G18">
+        <v>1250.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>45078</v>
+      </c>
+      <c r="B19">
+        <v>0.27</v>
+      </c>
+      <c r="C19">
+        <v>80.5</v>
+      </c>
+      <c r="D19">
+        <v>30</v>
+      </c>
+      <c r="E19">
+        <v>540</v>
+      </c>
+      <c r="F19">
+        <v>350</v>
+      </c>
+      <c r="G19">
+        <v>1280.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>45108</v>
+      </c>
+      <c r="B20">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C20">
+        <v>70</v>
+      </c>
+      <c r="D20">
+        <v>30.5</v>
+      </c>
+      <c r="E20">
+        <v>560.20000000000005</v>
+      </c>
+      <c r="F20">
+        <v>360.2</v>
+      </c>
+      <c r="G20">
+        <v>1300.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>45139</v>
+      </c>
+      <c r="B21">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C21">
+        <v>60.3</v>
+      </c>
+      <c r="D21">
+        <v>31</v>
+      </c>
+      <c r="E21">
+        <v>580.5</v>
+      </c>
+      <c r="F21">
+        <v>370.5</v>
+      </c>
+      <c r="G21">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>45170</v>
+      </c>
+      <c r="B22">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C22">
+        <v>90</v>
+      </c>
+      <c r="D22">
+        <v>30</v>
+      </c>
+      <c r="E22">
+        <v>550</v>
+      </c>
+      <c r="F22">
+        <v>355</v>
+      </c>
+      <c r="G22">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>45200</v>
+      </c>
+      <c r="B23">
+        <v>0.26</v>
+      </c>
+      <c r="C23">
+        <v>120.5</v>
+      </c>
+      <c r="D23">
+        <v>29</v>
+      </c>
+      <c r="E23">
+        <v>520.5</v>
+      </c>
+      <c r="F23">
+        <v>340.5</v>
+      </c>
+      <c r="G23">
+        <v>1250.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>45231</v>
+      </c>
+      <c r="B24">
+        <v>0.25</v>
+      </c>
+      <c r="C24">
+        <v>150</v>
+      </c>
+      <c r="D24">
+        <v>28</v>
+      </c>
+      <c r="E24">
+        <v>490</v>
+      </c>
+      <c r="F24">
+        <v>325</v>
+      </c>
+      <c r="G24">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>45261</v>
+      </c>
+      <c r="B25">
+        <v>0.24</v>
+      </c>
+      <c r="C25">
+        <v>180.3</v>
+      </c>
+      <c r="D25">
+        <v>27</v>
+      </c>
+      <c r="E25">
+        <v>460.5</v>
+      </c>
+      <c r="F25">
+        <v>310.3</v>
+      </c>
+      <c r="G25">
+        <v>1180.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>44927</v>
+      </c>
+      <c r="B26">
+        <v>0.23</v>
+      </c>
+      <c r="C26">
+        <v>200.1</v>
+      </c>
+      <c r="D26">
+        <v>27.5</v>
+      </c>
+      <c r="E26">
+        <v>420.5</v>
+      </c>
+      <c r="F26">
+        <v>280.3</v>
+      </c>
+      <c r="G26">
+        <v>1150.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>44958</v>
+      </c>
+      <c r="B27">
+        <v>0.22</v>
+      </c>
+      <c r="C27">
+        <v>180.5</v>
+      </c>
+      <c r="D27">
+        <v>28</v>
+      </c>
+      <c r="E27">
+        <v>450.7</v>
+      </c>
+      <c r="F27">
+        <v>300.5</v>
+      </c>
+      <c r="G27">
+        <v>1180.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>44986</v>
+      </c>
+      <c r="B28">
+        <v>0.24</v>
+      </c>
+      <c r="C28">
+        <v>150</v>
+      </c>
+      <c r="D28">
+        <v>28.5</v>
+      </c>
+      <c r="E28">
+        <v>480.2</v>
+      </c>
+      <c r="F28">
+        <v>320</v>
+      </c>
+      <c r="G28">
+        <v>1200.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>45017</v>
+      </c>
+      <c r="B29">
+        <v>0.25</v>
+      </c>
+      <c r="C29">
+        <v>120.3</v>
+      </c>
+      <c r="D29">
+        <v>29</v>
+      </c>
+      <c r="E29">
+        <v>500</v>
+      </c>
+      <c r="F29">
+        <v>330.2</v>
+      </c>
+      <c r="G29">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>45047</v>
+      </c>
+      <c r="B30">
+        <v>0.26</v>
+      </c>
+      <c r="C30">
+        <v>100</v>
+      </c>
+      <c r="D30">
+        <v>29.5</v>
+      </c>
+      <c r="E30">
+        <v>520.5</v>
+      </c>
+      <c r="F30">
+        <v>340.5</v>
+      </c>
+      <c r="G30">
+        <v>1250.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>45078</v>
+      </c>
+      <c r="B31">
+        <v>0.27</v>
+      </c>
+      <c r="C31">
+        <v>80.5</v>
+      </c>
+      <c r="D31">
+        <v>30</v>
+      </c>
+      <c r="E31">
+        <v>540</v>
+      </c>
+      <c r="F31">
+        <v>350</v>
+      </c>
+      <c r="G31">
+        <v>1280.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>45108</v>
+      </c>
+      <c r="B32">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C32">
+        <v>70</v>
+      </c>
+      <c r="D32">
+        <v>30.5</v>
+      </c>
+      <c r="E32">
+        <v>560.20000000000005</v>
+      </c>
+      <c r="F32">
+        <v>360.2</v>
+      </c>
+      <c r="G32">
+        <v>1300.7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>45139</v>
+      </c>
+      <c r="B33">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C33">
+        <v>60.3</v>
+      </c>
+      <c r="D33">
+        <v>31</v>
+      </c>
+      <c r="E33">
+        <v>580.5</v>
+      </c>
+      <c r="F33">
+        <v>370.5</v>
+      </c>
+      <c r="G33">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>45170</v>
+      </c>
+      <c r="B34">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C34">
+        <v>90</v>
+      </c>
+      <c r="D34">
+        <v>30</v>
+      </c>
+      <c r="E34">
+        <v>550</v>
+      </c>
+      <c r="F34">
+        <v>355</v>
+      </c>
+      <c r="G34">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>45200</v>
+      </c>
+      <c r="B35">
+        <v>0.26</v>
+      </c>
+      <c r="C35">
+        <v>120.5</v>
+      </c>
+      <c r="D35">
+        <v>29</v>
+      </c>
+      <c r="E35">
+        <v>520.5</v>
+      </c>
+      <c r="F35">
+        <v>340.5</v>
+      </c>
+      <c r="G35">
+        <v>1250.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>45231</v>
+      </c>
+      <c r="B36">
+        <v>0.25</v>
+      </c>
+      <c r="C36">
+        <v>150</v>
+      </c>
+      <c r="D36">
+        <v>28</v>
+      </c>
+      <c r="E36">
+        <v>490</v>
+      </c>
+      <c r="F36">
+        <v>325</v>
+      </c>
+      <c r="G36">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>45261</v>
+      </c>
+      <c r="B37">
+        <v>0.24</v>
+      </c>
+      <c r="C37">
+        <v>180.3</v>
+      </c>
+      <c r="D37">
+        <v>27</v>
+      </c>
+      <c r="E37">
+        <v>460.5</v>
+      </c>
+      <c r="F37">
+        <v>310.3</v>
+      </c>
+      <c r="G37">
+        <v>1180.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>